<commit_message>
Adding setNotificationHandler in App.js
</commit_message>
<xml_diff>
--- a/Back-end/files/FOLS.xlsx
+++ b/Back-end/files/FOLS.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosantos\OneDrive - Embraer\Desktop\FSE\FATEC\eFOL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lelen\Documents\GitHub\BriskNotificationApp\Back-end\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="478" documentId="8_{B5E5EBED-2410-4B4F-B3A6-A316E0F13876}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{1CF8F743-E8B9-4235-8AC5-4B2EF7F1EE4F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBC5758-1B3F-4FC2-BBE3-87D3D0A9E9A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="query" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="query" localSheetId="0" hidden="1">query!$A$1:$K$290</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2001" uniqueCount="762">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2016" uniqueCount="762">
   <si>
     <t>Title</t>
   </si>
@@ -2466,7 +2467,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2646,8 +2647,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -2762,6 +2769,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2807,7 +2825,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2815,50 +2833,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bom" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Célula de Verificação" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Célula Vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Ênfase1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Ênfase2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Ênfase3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Ênfase4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Ênfase5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Ênfase6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Neutro" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Ruim" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Saída" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de Aviso" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto Explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Título 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
@@ -2947,7 +2968,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_query" displayName="Table_query" ref="A1:K290" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:K290" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A2:K290">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K290">
     <sortCondition ref="G1:G290"/>
   </sortState>
   <tableColumns count="11">
@@ -2968,7 +2989,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3266,8 +3287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K290"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="D215" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12502,4 +12523,104 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C4A119C-E0F0-4351-A3C7-51A29A987DB3}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="B2" s="8"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>325</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A16">
+    <sortCondition ref="A1:A16"/>
+  </sortState>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>